<commit_message>
Předělány výrazy (už i trochu generují kód) + přidány common funkce
</commit_message>
<xml_diff>
--- a/doc/Tabulka výrazů.xlsx
+++ b/doc/Tabulka výrazů.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db9ed18a89a98c93/Dokumenty/VysokaSkola/IFJ/Projekt/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{72CB3A22-ED6C-41D9-B08D-8EF40193B9AB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{3378EDC8-E4C2-4257-8CB7-8E7F143F9EFC}"/>
+  <xr:revisionPtr revIDLastSave="535" documentId="8_{72CB3A22-ED6C-41D9-B08D-8EF40193B9AB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{BC9096C6-494A-40F4-BF46-3E3BF86218AF}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13965" xr2:uid="{670EBCC3-BF72-4DAF-A40A-916233B26669}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="25">
   <si>
     <t>+</t>
   </si>
@@ -88,6 +88,24 @@
   </si>
   <si>
     <t>Minified</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>not*</t>
+  </si>
+  <si>
+    <t>and,or*</t>
+  </si>
+  <si>
+    <t>* rozšíření boolop</t>
   </si>
 </sst>
 </file>
@@ -155,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -387,11 +405,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -445,15 +485,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -770,32 +828,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054048B2-AB80-4D3B-A113-B628E326B7E3}">
-  <dimension ref="C3:AB22"/>
+  <dimension ref="C3:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="17" width="4.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="3" max="20" width="4.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" customWidth="1"/>
+    <col min="25" max="35" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:28" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T3" s="20" t="s">
+    <row r="3" spans="3:35" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
     </row>
-    <row r="4" spans="3:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:35" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="10" t="s">
         <v>0</v>
@@ -828,45 +889,60 @@
         <v>7</v>
       </c>
       <c r="N4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="R4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="S4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="T4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="22"/>
-      <c r="U4" s="10" t="str">
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="10" t="str">
         <f>"+ -"</f>
         <v>+ -</v>
       </c>
-      <c r="V4" s="11" t="s">
+      <c r="AA4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="11" t="s">
+      <c r="AB4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="11" t="s">
+      <c r="AC4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Y4" s="11" t="s">
+      <c r="AD4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="11" t="s">
+      <c r="AG4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AA4" s="11" t="s">
+      <c r="AH4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AB4" s="13" t="s">
+      <c r="AI4" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>0</v>
       </c>
@@ -900,48 +976,59 @@
       <c r="M5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="N5" s="3"/>
       <c r="O5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="T5" s="14" t="str">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y5" s="14" t="str">
         <f>"+ -"</f>
         <v>+ -</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z5" s="3" t="s">
+      <c r="Z5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AB5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
         <v>1</v>
       </c>
@@ -975,47 +1062,58 @@
       <c r="M6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="N6" s="6"/>
       <c r="O6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="U6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z6" s="6" t="s">
+      <c r="Z6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
@@ -1049,45 +1147,58 @@
       <c r="M7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="N7" s="6"/>
       <c r="O7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="U7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>9</v>
+      <c r="Z7" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="AA7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AB7" s="7" t="s">
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="15" t="s">
         <v>3</v>
       </c>
@@ -1121,45 +1232,58 @@
       <c r="M8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="N8" s="6"/>
       <c r="O8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="U8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="6" t="s">
-        <v>9</v>
+      <c r="Z8" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="AA8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AB8" s="7" t="s">
+      <c r="AB8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
         <v>8</v>
       </c>
@@ -1192,38 +1316,55 @@
         <v>9</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB9" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z9" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI9" s="24" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="10" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="15" t="s">
         <v>9</v>
       </c>
@@ -1256,36 +1397,55 @@
         <v>9</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T10" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z10" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI10" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="16" t="s">
         <v>10</v>
       </c>
@@ -1318,36 +1478,53 @@
         <v>9</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="7" t="s">
-        <v>9</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD11" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE11" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI11" s="7"/>
     </row>
-    <row r="12" spans="3:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="15" t="s">
         <v>11</v>
       </c>
@@ -1380,36 +1557,49 @@
         <v>9</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T12" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="V12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="W12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="X12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB12" s="23"/>
+        <v>9</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="13" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="16" t="s">
         <v>6</v>
       </c>
@@ -1446,13 +1636,49 @@
         <v>9</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:35" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="15" t="s">
         <v>7</v>
       </c>
@@ -1489,209 +1715,461 @@
         <v>9</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>9</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD14" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE14" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI14" s="26"/>
     </row>
-    <row r="15" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="3:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y16" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="27"/>
+    </row>
+    <row r="17" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O15" s="6" t="s">
+      <c r="D18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q15" s="7"/>
+      <c r="S18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T18" s="7"/>
     </row>
-    <row r="16" spans="3:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="15" t="s">
+    <row r="19" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="7" t="s">
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S19" s="6"/>
+      <c r="T19" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="3:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="15" t="s">
+    <row r="20" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="7" t="s">
+      <c r="D20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S20" s="6"/>
+      <c r="T20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="3:17" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="17" t="s">
+    <row r="21" spans="3:20" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q18" s="19"/>
+      <c r="D21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="T21" s="26"/>
     </row>
-    <row r="19" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="18"/>
+    <row r="22" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="18"/>
     </row>
-    <row r="22" spans="3:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
+    <row r="23" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
     </row>
+    <row r="26" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="3:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="T3:AB3"/>
+  <mergeCells count="2">
+    <mergeCell ref="Y3:AI3"/>
+    <mergeCell ref="Y16:AB16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>